<commit_message>
[Pipette] Battery CON 검토 Part 추가
</commit_message>
<xml_diff>
--- a/1_Plasma_Pipette/1_Schematic/Plasma_Gen_Pipette_Main_BOM_V1.0_20180329.xlsx
+++ b/1_Plasma_Pipette/1_Schematic/Plasma_Gen_Pipette_Main_BOM_V1.0_20180329.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_Work\20171116_Plasma_Generator\1_Plasma_Pipette\1_Schematic\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12645"/>
   </bookViews>
@@ -17,12 +12,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0">Plasma_Pipette_Main_V1.0!$B$4:$L$4</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="255">
   <si>
     <t>No</t>
   </si>
@@ -805,6 +800,30 @@
   </si>
   <si>
     <t>BZT52C5V1S</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>009155003003016</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>Battery CON</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>AVX</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>3-Pin Battery Connector</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> P001217183 </t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>견적 요청</t>
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
 </sst>
@@ -1197,7 +1216,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -1586,6 +1605,51 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1719,7 +1783,7 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1904,6 +1968,18 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="43" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" quotePrefix="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2009,7 +2085,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2044,7 +2120,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2221,7 +2297,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2229,10 +2305,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V45"/>
+  <dimension ref="A1:V47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P26" sqref="P26"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I52" sqref="I52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4674,6 +4750,46 @@
       <c r="D45" s="3"/>
       <c r="N45"/>
     </row>
+    <row r="46" spans="1:22" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="47" spans="1:22" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B47" s="62"/>
+      <c r="C47" s="63" t="s">
+        <v>250</v>
+      </c>
+      <c r="D47" s="64" t="s">
+        <v>249</v>
+      </c>
+      <c r="E47" s="63" t="s">
+        <v>251</v>
+      </c>
+      <c r="F47" s="63"/>
+      <c r="G47" s="63" t="s">
+        <v>252</v>
+      </c>
+      <c r="H47" s="63">
+        <v>1</v>
+      </c>
+      <c r="I47" s="63"/>
+      <c r="J47" s="63"/>
+      <c r="K47" s="63"/>
+      <c r="L47" s="63"/>
+      <c r="M47" s="63"/>
+      <c r="N47" s="63"/>
+      <c r="O47" s="63"/>
+      <c r="P47" s="63"/>
+      <c r="Q47" s="63"/>
+      <c r="R47" s="63">
+        <v>10</v>
+      </c>
+      <c r="S47" s="63"/>
+      <c r="T47" s="63"/>
+      <c r="U47" s="63" t="s">
+        <v>253</v>
+      </c>
+      <c r="V47" s="65" t="s">
+        <v>254</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="B4:L4"/>
   <sortState ref="A19:AB40">

</xml_diff>